<commit_message>
working on create_db. making it read ranges dinamically
</commit_message>
<xml_diff>
--- a/Copy_of_updated_Hardware2.xlsx
+++ b/Copy_of_updated_Hardware2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\speard\Documents\Moorings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mackayp\moordesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BBFBB29-6E6B-4B56-9BD7-B0AF1DB5234F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40B8B3C-453F-474E-9C83-207B8779CADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{4E9EA262-9DA5-4196-B65F-CFA2DC6E9F4D}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{4E9EA262-9DA5-4196-B65F-CFA2DC6E9F4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -544,7 +544,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -578,6 +578,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -794,9 +802,6 @@
     <xf numFmtId="2" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -856,6 +861,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1174,20 +1182,18 @@
   <dimension ref="A1:I96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12:F14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.765625" customWidth="1"/>
-    <col min="4" max="5" width="12.765625" customWidth="1"/>
+    <col min="1" max="1" width="30.77734375" customWidth="1"/>
+    <col min="4" max="5" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
-        <v>19</v>
-      </c>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
       <c r="B1" t="s">
         <v>73</v>
       </c>
@@ -1213,8 +1219,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A2" s="7"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
+        <v>19</v>
+      </c>
       <c r="B2" t="s">
         <v>71</v>
       </c>
@@ -1231,8 +1239,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="5">
@@ -1254,8 +1262,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="5">
@@ -1277,8 +1285,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="5">
@@ -1300,8 +1308,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="5">
@@ -1323,8 +1331,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="5">
@@ -1346,8 +1354,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="5">
@@ -1369,8 +1377,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="5">
@@ -1392,8 +1400,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="5">
@@ -1415,8 +1423,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="5">
@@ -1438,8 +1446,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="5">
@@ -1461,8 +1469,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="5">
@@ -1484,8 +1492,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
         <v>31</v>
       </c>
       <c r="B14" s="5">
@@ -1507,22 +1515,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A15" s="12"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
       <c r="B15" s="5"/>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="13"/>
+    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12"/>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="14" t="s">
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="15" t="s">
+    <row r="18" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="5">
@@ -1545,8 +1553,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="5">
@@ -1569,8 +1577,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A20" s="17" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B20" s="5">
@@ -1593,8 +1601,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="16" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="5">
@@ -1616,8 +1624,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A22" s="17" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B22" s="5">
@@ -1639,8 +1647,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B23" s="5">
@@ -1663,8 +1671,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="5">
@@ -1686,8 +1694,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="16" t="s">
         <v>40</v>
       </c>
       <c r="B25" s="5">
@@ -1710,8 +1718,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B26" s="5">
@@ -1734,8 +1742,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="18" t="s">
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="17" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="5">
@@ -1758,22 +1766,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A29" s="19"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="18"/>
       <c r="B29" s="5"/>
     </row>
-    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="19" t="s">
         <v>83</v>
       </c>
       <c r="B30" s="5"/>
     </row>
-    <row r="31" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="21" t="s">
+    <row r="31" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="5">
@@ -1795,8 +1803,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A32" s="22" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
         <v>82</v>
       </c>
       <c r="B32" s="5">
@@ -1818,8 +1826,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A33" s="22" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
         <v>44</v>
       </c>
       <c r="B33" s="5">
@@ -1841,8 +1849,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A34" s="22" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="21" t="s">
         <v>46</v>
       </c>
       <c r="B34" s="5">
@@ -1864,8 +1872,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A35" s="23" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="22" t="s">
         <v>51</v>
       </c>
       <c r="B35" s="5">
@@ -1887,8 +1895,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A36" s="23" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="5">
@@ -1910,8 +1918,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A37" s="23" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="22" t="s">
         <v>53</v>
       </c>
       <c r="B37" s="5">
@@ -1933,8 +1941,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A38" s="23" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B38" s="5">
@@ -1956,8 +1964,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A39" s="26" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="25" t="s">
         <v>87</v>
       </c>
       <c r="B39" s="5">
@@ -1980,8 +1988,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A40" s="23" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="22" t="s">
         <v>86</v>
       </c>
       <c r="B40" s="5">
@@ -2003,8 +2011,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A41" s="23" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="22" t="s">
         <v>55</v>
       </c>
       <c r="B41" s="5">
@@ -2026,8 +2034,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A42" s="23" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="22" t="s">
         <v>85</v>
       </c>
       <c r="B42" s="5">
@@ -2049,8 +2057,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A43" s="22" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="21" t="s">
         <v>56</v>
       </c>
       <c r="B43" s="5">
@@ -2072,8 +2080,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A44" s="22" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="21" t="s">
         <v>57</v>
       </c>
       <c r="B44" s="5">
@@ -2095,8 +2103,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A45" s="22" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="21" t="s">
         <v>58</v>
       </c>
       <c r="B45" s="5">
@@ -2118,8 +2126,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A46" s="27" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="26" t="s">
         <v>59</v>
       </c>
       <c r="B46" s="5">
@@ -2141,8 +2149,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A47" s="22" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="21" t="s">
         <v>60</v>
       </c>
       <c r="B47" s="5">
@@ -2164,8 +2172,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A48" s="27" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="26" t="s">
         <v>61</v>
       </c>
       <c r="B48" s="5">
@@ -2187,8 +2195,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A49" s="22" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="21" t="s">
         <v>62</v>
       </c>
       <c r="B49" s="5">
@@ -2210,8 +2218,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A50" s="22" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="21" t="s">
         <v>67</v>
       </c>
       <c r="B50" s="5">
@@ -2233,8 +2241,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A51" s="22" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="21" t="s">
         <v>68</v>
       </c>
       <c r="B51" s="5">
@@ -2256,8 +2264,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A52" s="22" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="21" t="s">
         <v>69</v>
       </c>
       <c r="B52" s="5">
@@ -2279,18 +2287,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A55" s="22" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="21" t="s">
         <v>84</v>
       </c>
       <c r="B55" s="5"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A56" s="22" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="21" t="s">
         <v>89</v>
       </c>
       <c r="B56" s="5">
@@ -2312,8 +2320,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A57" s="22" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="21" t="s">
         <v>90</v>
       </c>
       <c r="B57" s="5">
@@ -2335,8 +2343,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A58" s="22" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="21" t="s">
         <v>91</v>
       </c>
       <c r="B58" s="5">
@@ -2358,8 +2366,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A59" s="22" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="21" t="s">
         <v>92</v>
       </c>
       <c r="B59" s="5">
@@ -2381,8 +2389,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A60" s="23" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B60" s="5">
@@ -2404,22 +2412,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A63" s="31" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="30" t="s">
         <v>88</v>
       </c>
       <c r="B63" s="5"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A64" s="22" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="21" t="s">
         <v>70</v>
       </c>
       <c r="B64" s="5">
@@ -2441,8 +2449,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A65" s="24" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B65" s="5">
@@ -2464,8 +2472,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A66" s="23" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="22" t="s">
         <v>48</v>
       </c>
       <c r="B66" s="5">
@@ -2488,8 +2496,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A67" s="23" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B67" s="5">
@@ -2511,8 +2519,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A68" s="25" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="24" t="s">
         <v>50</v>
       </c>
       <c r="B68" s="5">
@@ -2534,8 +2542,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A69" s="22" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="21" t="s">
         <v>66</v>
       </c>
       <c r="B69" s="5">
@@ -2557,8 +2565,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A70" s="27" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="26" t="s">
         <v>63</v>
       </c>
       <c r="B70" s="5">
@@ -2580,8 +2588,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A71" s="22" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="21" t="s">
         <v>64</v>
       </c>
       <c r="B71" s="5">
@@ -2603,8 +2611,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A72" s="22" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="21" t="s">
         <v>65</v>
       </c>
       <c r="B72" s="5">
@@ -2626,33 +2634,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="5"/>
       <c r="B74" s="5"/>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A75" s="28"/>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" s="27"/>
       <c r="B75" s="5"/>
     </row>
-    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="29"/>
+    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="28"/>
       <c r="B76" s="5"/>
     </row>
-    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B77" s="5"/>
     </row>
-    <row r="78" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B78" s="30">
+      <c r="B78" s="29">
         <v>-8.6666666666666663E-3</v>
       </c>
       <c r="C78">
@@ -2671,11 +2679,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B79" s="30">
+      <c r="B79" s="29">
         <v>1.0886734693877536E-3</v>
       </c>
       <c r="C79">
@@ -2694,11 +2702,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B80" s="30">
+      <c r="B80" s="29">
         <v>-9.4964028776978408E-3</v>
       </c>
       <c r="C80">
@@ -2717,11 +2725,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B81" s="30">
+      <c r="B81" s="29">
         <v>-24.8794</v>
       </c>
       <c r="C81">
@@ -2740,11 +2748,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B82" s="30">
+      <c r="B82" s="29">
         <v>-0.34473355</v>
       </c>
       <c r="C82">
@@ -2763,11 +2771,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B83" s="30">
+      <c r="B83" s="29">
         <v>-0.260791895</v>
       </c>
       <c r="C83">
@@ -2786,11 +2794,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="30">
+      <c r="B84" s="29">
         <v>2.3142857142857123E-3</v>
       </c>
       <c r="C84">
@@ -2809,11 +2817,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B85" s="30">
+      <c r="B85" s="29">
         <v>3.2115957446808494E-2</v>
       </c>
       <c r="C85">
@@ -2832,11 +2840,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B86" s="30">
+      <c r="B86" s="29">
         <v>-3.875701754385965E-2</v>
       </c>
       <c r="C86">
@@ -2855,11 +2863,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B87" s="30">
+      <c r="B87" s="29">
         <v>-3.3305263157894741E-2</v>
       </c>
       <c r="C87">
@@ -2878,11 +2886,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B88" s="30">
+      <c r="B88" s="29">
         <v>3.6642857142857102E-2</v>
       </c>
       <c r="C88">
@@ -2901,11 +2909,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B89" s="30">
+      <c r="B89" s="29">
         <v>-2.7385964912280687E-2</v>
       </c>
       <c r="C89">
@@ -2924,11 +2932,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B90" s="30">
+      <c r="B90" s="29">
         <v>1.1510204081632636E-3</v>
       </c>
       <c r="C90">
@@ -2947,11 +2955,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B91" s="30">
+      <c r="B91" s="29">
         <v>1.1030612244897942E-3</v>
       </c>
       <c r="C91">
@@ -2970,11 +2978,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B92" s="30">
+      <c r="B92" s="29">
         <v>-7.9297101449275365E-3</v>
       </c>
       <c r="C92">
@@ -2993,11 +3001,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B93" s="30">
+      <c r="B93" s="29">
         <v>-1.2278260869565218E-2</v>
       </c>
       <c r="C93">
@@ -3016,11 +3024,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B94" s="30">
+      <c r="B94" s="29">
         <v>-1.5859420289855073E-2</v>
       </c>
       <c r="C94">
@@ -3039,11 +3047,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B95" s="30">
+      <c r="B95" s="29">
         <v>-3.1207246376811593E-2</v>
       </c>
       <c r="C95">
@@ -3062,11 +3070,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B96" s="30">
+      <c r="B96" s="29">
         <v>-4.5787681159420293E-2</v>
       </c>
       <c r="C96">

</xml_diff>